<commit_message>
RMA enhancements: ZIP-based checkbox extraction, new priority/status, return address features, and bug fixes
</commit_message>
<xml_diff>
--- a/uploads/reference-documents/BlankRMA.xlsx
+++ b/uploads/reference-documents/BlankRMA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M282412\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\35KBEY99\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CB2CEEB-3A66-4C65-8043-D45BD7897448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7050F185-2162-410F-8554-FAF04A42ACA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="748" xr2:uid="{C5E8F13F-52FE-406C-AE41-2C92495A5527}"/>
@@ -2714,6 +2714,193 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2741,6 +2928,251 @@
     <xf numFmtId="44" fontId="39" fillId="4" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2762,448 +3194,32 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -3214,21 +3230,44 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3243,45 +3282,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -6031,7 +6031,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D17"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -6062,38 +6062,38 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="143">
+      <c r="I2" s="245">
         <f ca="1">TODAY()</f>
-        <v>45779</v>
-      </c>
-      <c r="J2" s="143"/>
+        <v>45950</v>
+      </c>
+      <c r="J2" s="245"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="193"/>
+      <c r="B3" s="196"/>
+      <c r="C3" s="196"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="196"/>
+      <c r="F3" s="196"/>
+      <c r="G3" s="196"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="196"/>
+      <c r="J3" s="196"/>
+      <c r="K3" s="197"/>
     </row>
     <row r="4" spans="1:11" ht="12" customHeight="1">
       <c r="A4" s="73"/>
-      <c r="H4" s="194" t="s">
+      <c r="H4" s="198" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="194"/>
-      <c r="J4" s="220" t="s">
+      <c r="I4" s="198"/>
+      <c r="J4" s="222" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="221"/>
+      <c r="K4" s="223"/>
     </row>
     <row r="5" spans="1:11" ht="12" customHeight="1">
       <c r="A5" s="74"/>
@@ -6103,79 +6103,79 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="194" t="s">
+      <c r="H5" s="198" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="194"/>
-      <c r="J5" s="222" t="s">
+      <c r="I5" s="198"/>
+      <c r="J5" s="224" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="223"/>
+      <c r="K5" s="225"/>
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="213"/>
-      <c r="C6" s="214"/>
-      <c r="D6" s="203" t="s">
+      <c r="B6" s="217"/>
+      <c r="C6" s="168"/>
+      <c r="D6" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="203"/>
+      <c r="E6" s="207"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="204" t="s">
+      <c r="G6" s="208" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="205"/>
-      <c r="I6" s="205"/>
-      <c r="J6" s="206"/>
+      <c r="H6" s="209"/>
+      <c r="I6" s="209"/>
+      <c r="J6" s="210"/>
       <c r="K6" s="75"/>
     </row>
     <row r="7" spans="1:11" ht="16.5" customHeight="1">
       <c r="A7" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="215"/>
-      <c r="C7" s="216"/>
-      <c r="D7" s="214"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="168"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="200"/>
-      <c r="H7" s="201"/>
-      <c r="I7" s="201"/>
-      <c r="J7" s="202"/>
+      <c r="G7" s="204"/>
+      <c r="H7" s="205"/>
+      <c r="I7" s="205"/>
+      <c r="J7" s="206"/>
       <c r="K7" s="75"/>
     </row>
     <row r="8" spans="1:11" ht="12" customHeight="1">
       <c r="A8" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="217"/>
-      <c r="C8" s="218"/>
-      <c r="D8" s="219"/>
+      <c r="B8" s="219"/>
+      <c r="C8" s="220"/>
+      <c r="D8" s="221"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="210" t="s">
+      <c r="G8" s="214" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="211"/>
-      <c r="I8" s="211"/>
-      <c r="J8" s="212"/>
+      <c r="H8" s="215"/>
+      <c r="I8" s="215"/>
+      <c r="J8" s="216"/>
       <c r="K8" s="75"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="224"/>
-      <c r="C9" s="218"/>
-      <c r="D9" s="219"/>
+      <c r="B9" s="226"/>
+      <c r="C9" s="220"/>
+      <c r="D9" s="221"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="195"/>
-      <c r="H9" s="196"/>
-      <c r="I9" s="196"/>
-      <c r="J9" s="197"/>
+      <c r="G9" s="199"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="201"/>
       <c r="K9" s="75"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
@@ -6185,36 +6185,36 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="207" t="s">
+      <c r="G10" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="208"/>
-      <c r="I10" s="208"/>
-      <c r="J10" s="209"/>
+      <c r="H10" s="212"/>
+      <c r="I10" s="212"/>
+      <c r="J10" s="213"/>
       <c r="K10" s="75"/>
     </row>
     <row r="11" spans="1:11" ht="17.25" customHeight="1">
       <c r="A11" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="171"/>
-      <c r="C11" s="172"/>
-      <c r="D11" s="173"/>
+      <c r="B11" s="227"/>
+      <c r="C11" s="228"/>
+      <c r="D11" s="229"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="198"/>
-      <c r="H11" s="196"/>
-      <c r="I11" s="196"/>
-      <c r="J11" s="199"/>
+      <c r="G11" s="202"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="203"/>
       <c r="K11" s="75"/>
     </row>
     <row r="12" spans="1:11" ht="12" customHeight="1">
       <c r="A12" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="174"/>
-      <c r="C12" s="175"/>
-      <c r="D12" s="176"/>
+      <c r="B12" s="230"/>
+      <c r="C12" s="231"/>
+      <c r="D12" s="232"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="K12" s="75"/>
@@ -6223,112 +6223,112 @@
       <c r="A13" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="174"/>
-      <c r="C13" s="175"/>
-      <c r="D13" s="176"/>
+      <c r="B13" s="230"/>
+      <c r="C13" s="231"/>
+      <c r="D13" s="232"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="179" t="s">
+      <c r="F13" s="233" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="179"/>
-      <c r="H13" s="179"/>
-      <c r="I13" s="179"/>
-      <c r="J13" s="179"/>
-      <c r="K13" s="180"/>
+      <c r="G13" s="233"/>
+      <c r="H13" s="233"/>
+      <c r="I13" s="233"/>
+      <c r="J13" s="233"/>
+      <c r="K13" s="234"/>
     </row>
     <row r="14" spans="1:11" ht="12" customHeight="1">
       <c r="A14" s="80"/>
-      <c r="B14" s="174"/>
-      <c r="C14" s="175"/>
-      <c r="D14" s="176"/>
+      <c r="B14" s="230"/>
+      <c r="C14" s="231"/>
+      <c r="D14" s="232"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="181"/>
-      <c r="G14" s="182"/>
-      <c r="H14" s="182"/>
-      <c r="I14" s="182"/>
-      <c r="J14" s="182"/>
-      <c r="K14" s="183"/>
+      <c r="F14" s="235"/>
+      <c r="G14" s="236"/>
+      <c r="H14" s="236"/>
+      <c r="I14" s="236"/>
+      <c r="J14" s="236"/>
+      <c r="K14" s="237"/>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1">
       <c r="A15" s="80"/>
-      <c r="B15" s="174"/>
-      <c r="C15" s="175"/>
-      <c r="D15" s="176"/>
+      <c r="B15" s="230"/>
+      <c r="C15" s="231"/>
+      <c r="D15" s="232"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="144" t="s">
+      <c r="F15" s="246" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="144"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="144"/>
-      <c r="J15" s="144"/>
-      <c r="K15" s="145"/>
+      <c r="G15" s="246"/>
+      <c r="H15" s="246"/>
+      <c r="I15" s="246"/>
+      <c r="J15" s="246"/>
+      <c r="K15" s="247"/>
     </row>
     <row r="16" spans="1:11" ht="22.5" customHeight="1">
       <c r="A16" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="174"/>
-      <c r="C16" s="175"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="188" t="s">
+      <c r="B16" s="230"/>
+      <c r="C16" s="231"/>
+      <c r="D16" s="232"/>
+      <c r="E16" s="242" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="189"/>
-      <c r="G16" s="189"/>
-      <c r="H16" s="189"/>
-      <c r="I16" s="190"/>
-      <c r="J16" s="184"/>
-      <c r="K16" s="185"/>
+      <c r="F16" s="243"/>
+      <c r="G16" s="243"/>
+      <c r="H16" s="243"/>
+      <c r="I16" s="244"/>
+      <c r="J16" s="238"/>
+      <c r="K16" s="239"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="174"/>
-      <c r="C17" s="175"/>
-      <c r="D17" s="176"/>
+      <c r="B17" s="230"/>
+      <c r="C17" s="231"/>
+      <c r="D17" s="232"/>
       <c r="E17" s="5"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="177" t="s">
+      <c r="G17" s="160" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="177"/>
-      <c r="I17" s="177"/>
-      <c r="J17" s="186"/>
-      <c r="K17" s="187"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="240"/>
+      <c r="K17" s="241"/>
     </row>
     <row r="18" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A18" s="258" t="s">
+      <c r="A18" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="259"/>
-      <c r="C18" s="259"/>
-      <c r="D18" s="260"/>
+      <c r="B18" s="135"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="136"/>
       <c r="E18" s="5"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="177" t="s">
+      <c r="G18" s="160" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="177"/>
-      <c r="I18" s="177"/>
-      <c r="J18" s="187"/>
-      <c r="K18" s="187"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="160"/>
+      <c r="J18" s="241"/>
+      <c r="K18" s="241"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" customHeight="1">
       <c r="A19" s="98"/>
-      <c r="B19" s="261" t="s">
+      <c r="B19" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="261"/>
-      <c r="D19" s="262"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="138"/>
       <c r="E19" s="5"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="177" t="s">
+      <c r="G19" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="177"/>
-      <c r="I19" s="178"/>
+      <c r="H19" s="160"/>
+      <c r="I19" s="161"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
@@ -6339,11 +6339,11 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="177" t="s">
+      <c r="G20" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="177"/>
-      <c r="I20" s="178"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="161"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
     </row>
@@ -6354,45 +6354,45 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="177" t="s">
+      <c r="G21" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="177"/>
-      <c r="I21" s="178"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="161"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A22" s="236" t="s">
+      <c r="A22" s="162" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="237"/>
-      <c r="C22" s="237"/>
-      <c r="D22" s="237"/>
-      <c r="E22" s="237"/>
+      <c r="B22" s="163"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="163"/>
+      <c r="E22" s="163"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="244" t="s">
+      <c r="G22" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="244"/>
-      <c r="I22" s="245"/>
-      <c r="J22" s="246"/>
-      <c r="K22" s="247"/>
+      <c r="H22" s="169"/>
+      <c r="I22" s="170"/>
+      <c r="J22" s="171"/>
+      <c r="K22" s="172"/>
     </row>
     <row r="23" spans="1:11" ht="12" customHeight="1" thickBot="1">
-      <c r="A23" s="238" t="s">
+      <c r="A23" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="239"/>
-      <c r="C23" s="239"/>
-      <c r="D23" s="239"/>
-      <c r="E23" s="239"/>
-      <c r="F23" s="239"/>
-      <c r="G23" s="239"/>
-      <c r="H23" s="239"/>
-      <c r="I23" s="239"/>
-      <c r="J23" s="239"/>
-      <c r="K23" s="240"/>
+      <c r="B23" s="165"/>
+      <c r="C23" s="165"/>
+      <c r="D23" s="165"/>
+      <c r="E23" s="165"/>
+      <c r="F23" s="165"/>
+      <c r="G23" s="165"/>
+      <c r="H23" s="165"/>
+      <c r="I23" s="165"/>
+      <c r="J23" s="165"/>
+      <c r="K23" s="166"/>
     </row>
     <row r="24" spans="1:11" ht="12" customHeight="1">
       <c r="A24" s="101" t="s">
@@ -6415,52 +6415,52 @@
       <c r="A25" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="215"/>
-      <c r="C25" s="214"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="168"/>
       <c r="D25" s="105"/>
       <c r="E25" s="111"/>
-      <c r="F25" s="248" t="s">
+      <c r="F25" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="249"/>
-      <c r="H25" s="249"/>
-      <c r="I25" s="250"/>
-      <c r="J25" s="215"/>
-      <c r="K25" s="214"/>
+      <c r="G25" s="174"/>
+      <c r="H25" s="174"/>
+      <c r="I25" s="175"/>
+      <c r="J25" s="167"/>
+      <c r="K25" s="168"/>
     </row>
     <row r="26" spans="1:11" ht="13.5" customHeight="1">
       <c r="A26" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="168"/>
-      <c r="C26" s="169"/>
-      <c r="D26" s="170"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="156"/>
+      <c r="D26" s="157"/>
       <c r="E26" s="111"/>
       <c r="F26" s="76" t="s">
         <v>36</v>
       </c>
       <c r="G26" s="106"/>
       <c r="H26" s="106"/>
-      <c r="I26" s="168"/>
-      <c r="J26" s="169"/>
-      <c r="K26" s="170"/>
+      <c r="I26" s="155"/>
+      <c r="J26" s="156"/>
+      <c r="K26" s="157"/>
     </row>
     <row r="27" spans="1:11" ht="12" customHeight="1">
       <c r="A27" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="241"/>
-      <c r="C27" s="242"/>
-      <c r="D27" s="243"/>
+      <c r="B27" s="145"/>
+      <c r="C27" s="146"/>
+      <c r="D27" s="147"/>
       <c r="E27" s="111"/>
       <c r="F27" s="109" t="s">
         <v>38</v>
       </c>
       <c r="G27" s="110"/>
       <c r="H27" s="110"/>
-      <c r="I27" s="241"/>
-      <c r="J27" s="242"/>
-      <c r="K27" s="243"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="146"/>
+      <c r="K27" s="147"/>
     </row>
     <row r="28" spans="1:11" ht="2.25" customHeight="1">
       <c r="A28" s="113"/>
@@ -6479,16 +6479,16 @@
       <c r="A29" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="241"/>
-      <c r="C29" s="242"/>
-      <c r="D29" s="243"/>
+      <c r="B29" s="145"/>
+      <c r="C29" s="146"/>
+      <c r="D29" s="147"/>
       <c r="E29" s="111"/>
-      <c r="F29" s="251" t="s">
+      <c r="F29" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="252"/>
-      <c r="H29" s="252"/>
-      <c r="I29" s="253"/>
+      <c r="G29" s="177"/>
+      <c r="H29" s="177"/>
+      <c r="I29" s="178"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
     </row>
@@ -6496,8 +6496,8 @@
       <c r="A30" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="215"/>
-      <c r="C30" s="214"/>
+      <c r="B30" s="167"/>
+      <c r="C30" s="168"/>
       <c r="D30" s="75"/>
       <c r="E30" s="111"/>
       <c r="F30" s="76" t="s">
@@ -6506,57 +6506,57 @@
       <c r="G30" s="106"/>
       <c r="H30" s="106"/>
       <c r="I30" s="82"/>
-      <c r="J30" s="215"/>
-      <c r="K30" s="214"/>
+      <c r="J30" s="167"/>
+      <c r="K30" s="168"/>
     </row>
     <row r="31" spans="1:11" ht="12" customHeight="1">
       <c r="A31" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="168"/>
-      <c r="C31" s="169"/>
-      <c r="D31" s="170"/>
+      <c r="B31" s="155"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="157"/>
       <c r="E31" s="111"/>
       <c r="F31" s="76" t="s">
         <v>36</v>
       </c>
       <c r="G31" s="106"/>
       <c r="H31" s="106"/>
-      <c r="I31" s="168"/>
-      <c r="J31" s="169"/>
-      <c r="K31" s="170"/>
+      <c r="I31" s="155"/>
+      <c r="J31" s="156"/>
+      <c r="K31" s="157"/>
     </row>
     <row r="32" spans="1:11" ht="13.5" customHeight="1" thickBot="1">
       <c r="A32" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="241"/>
-      <c r="C32" s="242"/>
-      <c r="D32" s="243"/>
+      <c r="B32" s="145"/>
+      <c r="C32" s="146"/>
+      <c r="D32" s="147"/>
       <c r="E32" s="111"/>
       <c r="F32" s="107" t="s">
         <v>38</v>
       </c>
       <c r="G32" s="83"/>
       <c r="H32" s="83"/>
-      <c r="I32" s="263"/>
-      <c r="J32" s="264"/>
-      <c r="K32" s="265"/>
+      <c r="I32" s="148"/>
+      <c r="J32" s="149"/>
+      <c r="K32" s="150"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A33" s="266" t="s">
+      <c r="A33" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="267"/>
-      <c r="C33" s="267"/>
-      <c r="D33" s="267"/>
-      <c r="E33" s="267"/>
-      <c r="F33" s="268"/>
-      <c r="G33" s="268"/>
-      <c r="H33" s="268"/>
-      <c r="I33" s="268"/>
-      <c r="J33" s="268"/>
-      <c r="K33" s="269"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="153"/>
+      <c r="G33" s="153"/>
+      <c r="H33" s="153"/>
+      <c r="I33" s="153"/>
+      <c r="J33" s="153"/>
+      <c r="K33" s="154"/>
     </row>
     <row r="34" spans="1:11" ht="19.5" customHeight="1">
       <c r="A34" s="70" t="s">
@@ -6564,19 +6564,19 @@
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
-      <c r="D34" s="254" t="str">
+      <c r="D34" s="130" t="str">
         <f>IF(Data!A21=TRUE,HYPERLINK(Data!A29, Data!B29),IF(Data!A25=TRUE,HYPERLINK(Data!A29, Data!B29)," "))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E34" s="255"/>
-      <c r="F34" s="156" t="s">
+      <c r="E34" s="131"/>
+      <c r="F34" s="258" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="157"/>
-      <c r="H34" s="157"/>
-      <c r="I34" s="157"/>
-      <c r="J34" s="157"/>
-      <c r="K34" s="158"/>
+      <c r="G34" s="259"/>
+      <c r="H34" s="259"/>
+      <c r="I34" s="259"/>
+      <c r="J34" s="259"/>
+      <c r="K34" s="260"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="71" t="s">
@@ -6584,92 +6584,92 @@
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
-      <c r="D35" s="256"/>
-      <c r="E35" s="257"/>
-      <c r="F35" s="159" t="str">
+      <c r="D35" s="132"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="261" t="str">
         <f>IF(Data!A21=TRUE,"PURGING AND DOUBLE BAGGING REQUIRED",IF(Data!A22=TRUE,"N/A-Not Exposed",""))</f>
         <v/>
       </c>
-      <c r="G35" s="160"/>
-      <c r="H35" s="160"/>
-      <c r="I35" s="160"/>
-      <c r="J35" s="160"/>
-      <c r="K35" s="161"/>
+      <c r="G35" s="262"/>
+      <c r="H35" s="262"/>
+      <c r="I35" s="262"/>
+      <c r="J35" s="262"/>
+      <c r="K35" s="263"/>
     </row>
     <row r="36" spans="1:11" ht="24.75" customHeight="1">
       <c r="A36" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="153"/>
-      <c r="C36" s="154"/>
-      <c r="D36" s="154"/>
-      <c r="E36" s="154"/>
-      <c r="F36" s="154"/>
-      <c r="G36" s="154"/>
-      <c r="H36" s="154"/>
-      <c r="I36" s="154"/>
-      <c r="J36" s="154"/>
-      <c r="K36" s="155"/>
+      <c r="B36" s="255"/>
+      <c r="C36" s="256"/>
+      <c r="D36" s="256"/>
+      <c r="E36" s="256"/>
+      <c r="F36" s="256"/>
+      <c r="G36" s="256"/>
+      <c r="H36" s="256"/>
+      <c r="I36" s="256"/>
+      <c r="J36" s="256"/>
+      <c r="K36" s="257"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A37" s="162" t="s">
+      <c r="A37" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="163"/>
-      <c r="C37" s="163"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="163"/>
-      <c r="F37" s="163"/>
-      <c r="G37" s="163"/>
-      <c r="H37" s="163"/>
-      <c r="I37" s="163"/>
-      <c r="J37" s="163"/>
-      <c r="K37" s="164"/>
+      <c r="B37" s="143"/>
+      <c r="C37" s="143"/>
+      <c r="D37" s="143"/>
+      <c r="E37" s="143"/>
+      <c r="F37" s="143"/>
+      <c r="G37" s="143"/>
+      <c r="H37" s="143"/>
+      <c r="I37" s="143"/>
+      <c r="J37" s="143"/>
+      <c r="K37" s="144"/>
     </row>
     <row r="38" spans="1:11" ht="21.75" customHeight="1">
       <c r="A38" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="165"/>
-      <c r="C38" s="166"/>
-      <c r="D38" s="166"/>
-      <c r="E38" s="166"/>
-      <c r="F38" s="166"/>
-      <c r="G38" s="166"/>
-      <c r="H38" s="166"/>
-      <c r="I38" s="166"/>
-      <c r="J38" s="166"/>
-      <c r="K38" s="167"/>
+      <c r="B38" s="139"/>
+      <c r="C38" s="140"/>
+      <c r="D38" s="140"/>
+      <c r="E38" s="140"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="140"/>
+      <c r="I38" s="140"/>
+      <c r="J38" s="140"/>
+      <c r="K38" s="141"/>
     </row>
     <row r="39" spans="1:11" ht="30" customHeight="1">
       <c r="A39" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="165"/>
-      <c r="C39" s="166"/>
-      <c r="D39" s="166"/>
-      <c r="E39" s="166"/>
-      <c r="F39" s="166"/>
-      <c r="G39" s="166"/>
-      <c r="H39" s="166"/>
-      <c r="I39" s="166"/>
-      <c r="J39" s="166"/>
-      <c r="K39" s="167"/>
+      <c r="B39" s="139"/>
+      <c r="C39" s="140"/>
+      <c r="D39" s="140"/>
+      <c r="E39" s="140"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="140"/>
+      <c r="I39" s="140"/>
+      <c r="J39" s="140"/>
+      <c r="K39" s="141"/>
     </row>
     <row r="40" spans="1:11" ht="136.5" customHeight="1">
       <c r="A40" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="165"/>
-      <c r="C40" s="166"/>
-      <c r="D40" s="166"/>
-      <c r="E40" s="166"/>
-      <c r="F40" s="166"/>
-      <c r="G40" s="166"/>
-      <c r="H40" s="166"/>
-      <c r="I40" s="166"/>
-      <c r="J40" s="166"/>
-      <c r="K40" s="167"/>
+      <c r="B40" s="139"/>
+      <c r="C40" s="140"/>
+      <c r="D40" s="140"/>
+      <c r="E40" s="140"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="140"/>
+      <c r="I40" s="140"/>
+      <c r="J40" s="140"/>
+      <c r="K40" s="141"/>
     </row>
     <row r="41" spans="1:11" ht="19.5" customHeight="1" thickBot="1">
       <c r="A41" s="88"/>
@@ -6685,134 +6685,134 @@
       <c r="K41" s="99"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A42" s="162" t="s">
+      <c r="A42" s="142" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="163"/>
-      <c r="C42" s="163"/>
-      <c r="D42" s="163"/>
-      <c r="E42" s="163"/>
-      <c r="F42" s="163"/>
-      <c r="G42" s="163"/>
-      <c r="H42" s="163"/>
-      <c r="I42" s="163"/>
-      <c r="J42" s="163"/>
-      <c r="K42" s="164"/>
+      <c r="B42" s="143"/>
+      <c r="C42" s="143"/>
+      <c r="D42" s="143"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="143"/>
+      <c r="G42" s="143"/>
+      <c r="H42" s="143"/>
+      <c r="I42" s="143"/>
+      <c r="J42" s="143"/>
+      <c r="K42" s="144"/>
     </row>
     <row r="43" spans="1:11" ht="12.75" customHeight="1">
       <c r="A43" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="137"/>
-      <c r="C43" s="138"/>
-      <c r="D43" s="138"/>
-      <c r="E43" s="138"/>
-      <c r="F43" s="138"/>
-      <c r="G43" s="138"/>
-      <c r="H43" s="138"/>
-      <c r="I43" s="138"/>
-      <c r="J43" s="138"/>
-      <c r="K43" s="139"/>
+      <c r="B43" s="264"/>
+      <c r="C43" s="265"/>
+      <c r="D43" s="265"/>
+      <c r="E43" s="265"/>
+      <c r="F43" s="265"/>
+      <c r="G43" s="265"/>
+      <c r="H43" s="265"/>
+      <c r="I43" s="265"/>
+      <c r="J43" s="265"/>
+      <c r="K43" s="266"/>
     </row>
     <row r="44" spans="1:11" ht="253.5" customHeight="1">
       <c r="A44" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="140"/>
-      <c r="C44" s="141"/>
-      <c r="D44" s="141"/>
-      <c r="E44" s="141"/>
-      <c r="F44" s="141"/>
-      <c r="G44" s="141"/>
-      <c r="H44" s="141"/>
-      <c r="I44" s="141"/>
-      <c r="J44" s="141"/>
-      <c r="K44" s="142"/>
+      <c r="B44" s="267"/>
+      <c r="C44" s="268"/>
+      <c r="D44" s="268"/>
+      <c r="E44" s="268"/>
+      <c r="F44" s="268"/>
+      <c r="G44" s="268"/>
+      <c r="H44" s="268"/>
+      <c r="I44" s="268"/>
+      <c r="J44" s="268"/>
+      <c r="K44" s="269"/>
     </row>
     <row r="45" spans="1:11" ht="12" customHeight="1">
-      <c r="A45" s="228" t="s">
+      <c r="A45" s="182" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="229"/>
-      <c r="C45" s="229"/>
-      <c r="D45" s="229"/>
-      <c r="E45" s="229"/>
-      <c r="F45" s="229"/>
-      <c r="G45" s="229"/>
-      <c r="H45" s="229"/>
-      <c r="I45" s="229"/>
-      <c r="J45" s="229"/>
-      <c r="K45" s="230"/>
+      <c r="B45" s="183"/>
+      <c r="C45" s="183"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="183"/>
+      <c r="F45" s="183"/>
+      <c r="G45" s="183"/>
+      <c r="H45" s="183"/>
+      <c r="I45" s="183"/>
+      <c r="J45" s="183"/>
+      <c r="K45" s="184"/>
     </row>
     <row r="46" spans="1:11" ht="350.25" customHeight="1">
       <c r="A46" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="231"/>
-      <c r="C46" s="231"/>
-      <c r="D46" s="231"/>
-      <c r="E46" s="231"/>
-      <c r="F46" s="231"/>
-      <c r="G46" s="231"/>
-      <c r="H46" s="231"/>
-      <c r="I46" s="231"/>
-      <c r="J46" s="231"/>
-      <c r="K46" s="231"/>
+      <c r="B46" s="185"/>
+      <c r="C46" s="185"/>
+      <c r="D46" s="185"/>
+      <c r="E46" s="185"/>
+      <c r="F46" s="185"/>
+      <c r="G46" s="185"/>
+      <c r="H46" s="185"/>
+      <c r="I46" s="185"/>
+      <c r="J46" s="185"/>
+      <c r="K46" s="185"/>
     </row>
     <row r="47" spans="1:11" ht="30.75" customHeight="1">
       <c r="A47" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="231"/>
-      <c r="C47" s="231"/>
-      <c r="D47" s="231"/>
-      <c r="E47" s="231"/>
-      <c r="F47" s="231"/>
-      <c r="G47" s="231"/>
-      <c r="H47" s="231"/>
-      <c r="I47" s="231"/>
-      <c r="J47" s="231"/>
-      <c r="K47" s="231"/>
+      <c r="B47" s="185"/>
+      <c r="C47" s="185"/>
+      <c r="D47" s="185"/>
+      <c r="E47" s="185"/>
+      <c r="F47" s="185"/>
+      <c r="G47" s="185"/>
+      <c r="H47" s="185"/>
+      <c r="I47" s="185"/>
+      <c r="J47" s="185"/>
+      <c r="K47" s="185"/>
     </row>
     <row r="48" spans="1:11" ht="18" customHeight="1">
-      <c r="A48" s="146"/>
-      <c r="B48" s="146"/>
-      <c r="C48" s="146"/>
-      <c r="D48" s="146"/>
-      <c r="E48" s="146"/>
-      <c r="F48" s="146"/>
-      <c r="G48" s="146"/>
-      <c r="H48" s="146"/>
-      <c r="I48" s="146"/>
-      <c r="J48" s="146"/>
-      <c r="K48" s="146"/>
+      <c r="A48" s="248"/>
+      <c r="B48" s="248"/>
+      <c r="C48" s="248"/>
+      <c r="D48" s="248"/>
+      <c r="E48" s="248"/>
+      <c r="F48" s="248"/>
+      <c r="G48" s="248"/>
+      <c r="H48" s="248"/>
+      <c r="I48" s="248"/>
+      <c r="J48" s="248"/>
+      <c r="K48" s="248"/>
     </row>
     <row r="49" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A49" s="147" t="s">
+      <c r="A49" s="249" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="148"/>
-      <c r="C49" s="148"/>
-      <c r="D49" s="148"/>
-      <c r="E49" s="148"/>
-      <c r="F49" s="148"/>
-      <c r="G49" s="148"/>
-      <c r="H49" s="148"/>
-      <c r="I49" s="148"/>
-      <c r="J49" s="148"/>
-      <c r="K49" s="149"/>
+      <c r="B49" s="250"/>
+      <c r="C49" s="250"/>
+      <c r="D49" s="250"/>
+      <c r="E49" s="250"/>
+      <c r="F49" s="250"/>
+      <c r="G49" s="250"/>
+      <c r="H49" s="250"/>
+      <c r="I49" s="250"/>
+      <c r="J49" s="250"/>
+      <c r="K49" s="251"/>
     </row>
     <row r="50" spans="1:11" ht="12" customHeight="1">
-      <c r="A50" s="150" t="s">
+      <c r="A50" s="252" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="151"/>
-      <c r="C50" s="152"/>
-      <c r="D50" s="150" t="s">
+      <c r="B50" s="253"/>
+      <c r="C50" s="254"/>
+      <c r="D50" s="252" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="151"/>
-      <c r="F50" s="152"/>
+      <c r="E50" s="253"/>
+      <c r="F50" s="254"/>
       <c r="G50" s="91" t="s">
         <v>57</v>
       </c>
@@ -6822,90 +6822,90 @@
       <c r="I50" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="J50" s="232" t="s">
+      <c r="J50" s="193" t="s">
         <v>60</v>
       </c>
-      <c r="K50" s="232"/>
+      <c r="K50" s="193"/>
     </row>
     <row r="51" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A51" s="130"/>
-      <c r="B51" s="131"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="133"/>
-      <c r="E51" s="134"/>
-      <c r="F51" s="135"/>
+      <c r="A51" s="186"/>
+      <c r="B51" s="187"/>
+      <c r="C51" s="188"/>
+      <c r="D51" s="189"/>
+      <c r="E51" s="190"/>
+      <c r="F51" s="191"/>
       <c r="G51" s="95"/>
       <c r="H51" s="97"/>
       <c r="I51" s="96"/>
-      <c r="J51" s="136">
+      <c r="J51" s="192">
         <f>G51*I51</f>
         <v>0</v>
       </c>
-      <c r="K51" s="136"/>
+      <c r="K51" s="192"/>
     </row>
     <row r="52" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A52" s="130"/>
-      <c r="B52" s="131"/>
-      <c r="C52" s="132"/>
-      <c r="D52" s="133"/>
-      <c r="E52" s="134"/>
-      <c r="F52" s="135"/>
+      <c r="A52" s="186"/>
+      <c r="B52" s="187"/>
+      <c r="C52" s="188"/>
+      <c r="D52" s="189"/>
+      <c r="E52" s="190"/>
+      <c r="F52" s="191"/>
       <c r="G52" s="95"/>
       <c r="H52" s="95"/>
       <c r="I52" s="96"/>
-      <c r="J52" s="136">
+      <c r="J52" s="192">
         <f t="shared" ref="J52:J55" si="0">G52*I52</f>
         <v>0</v>
       </c>
-      <c r="K52" s="136"/>
+      <c r="K52" s="192"/>
     </row>
     <row r="53" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A53" s="130"/>
-      <c r="B53" s="131"/>
-      <c r="C53" s="132"/>
-      <c r="D53" s="133"/>
-      <c r="E53" s="134"/>
-      <c r="F53" s="135"/>
+      <c r="A53" s="186"/>
+      <c r="B53" s="187"/>
+      <c r="C53" s="188"/>
+      <c r="D53" s="189"/>
+      <c r="E53" s="190"/>
+      <c r="F53" s="191"/>
       <c r="G53" s="95"/>
       <c r="H53" s="95"/>
       <c r="I53" s="96"/>
-      <c r="J53" s="136">
+      <c r="J53" s="192">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K53" s="136"/>
+      <c r="K53" s="192"/>
     </row>
     <row r="54" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A54" s="130"/>
-      <c r="B54" s="131"/>
-      <c r="C54" s="132"/>
-      <c r="D54" s="133"/>
-      <c r="E54" s="134"/>
-      <c r="F54" s="135"/>
+      <c r="A54" s="186"/>
+      <c r="B54" s="187"/>
+      <c r="C54" s="188"/>
+      <c r="D54" s="189"/>
+      <c r="E54" s="190"/>
+      <c r="F54" s="191"/>
       <c r="G54" s="95"/>
       <c r="H54" s="95"/>
       <c r="I54" s="96"/>
-      <c r="J54" s="136">
+      <c r="J54" s="192">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K54" s="136"/>
+      <c r="K54" s="192"/>
     </row>
     <row r="55" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A55" s="130"/>
-      <c r="B55" s="131"/>
-      <c r="C55" s="132"/>
-      <c r="D55" s="133"/>
-      <c r="E55" s="134"/>
-      <c r="F55" s="135"/>
+      <c r="A55" s="186"/>
+      <c r="B55" s="187"/>
+      <c r="C55" s="188"/>
+      <c r="D55" s="189"/>
+      <c r="E55" s="190"/>
+      <c r="F55" s="191"/>
       <c r="G55" s="95"/>
       <c r="H55" s="95"/>
       <c r="I55" s="96"/>
-      <c r="J55" s="136">
+      <c r="J55" s="192">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K55" s="136"/>
+      <c r="K55" s="192"/>
     </row>
     <row r="56" spans="1:11" ht="16.5" customHeight="1">
       <c r="A56" s="92"/>
@@ -6915,15 +6915,15 @@
       <c r="E56" s="72"/>
       <c r="F56" s="72"/>
       <c r="G56" s="72"/>
-      <c r="H56" s="233" t="s">
+      <c r="H56" s="194" t="s">
         <v>61</v>
       </c>
-      <c r="I56" s="233"/>
-      <c r="J56" s="136">
+      <c r="I56" s="194"/>
+      <c r="J56" s="192">
         <f>SUM(J51:K55)</f>
         <v>0</v>
       </c>
-      <c r="K56" s="136"/>
+      <c r="K56" s="192"/>
     </row>
     <row r="57" spans="1:11" ht="16.5" customHeight="1">
       <c r="A57" s="92"/>
@@ -6939,9 +6939,9 @@
       <c r="K57" s="94"/>
     </row>
     <row r="58" spans="1:11" ht="12" customHeight="1">
-      <c r="A58" s="234"/>
-      <c r="B58" s="235"/>
-      <c r="C58" s="235"/>
+      <c r="A58" s="158"/>
+      <c r="B58" s="159"/>
+      <c r="C58" s="159"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -6955,15 +6955,15 @@
       <c r="A59" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="225" t="str">
+      <c r="B59" s="179" t="str">
         <f>HYPERLINK("mailto:"&amp;(IF(G9="","Select DSS Product line",IF(ISNUMBER(SEARCH("HYT",G9)),"VMHYTRMA",IF(ISNUMBER(SEARCH("KEEPER",G9)),"VMHYTRMA",IF(G9="GasStar","DSSCNRMA@merckgroup.com","DSSRMA@emdgroup.com"))))))</f>
         <v>mailto:Select DSS Product line</v>
       </c>
-      <c r="C59" s="226"/>
-      <c r="D59" s="226"/>
-      <c r="E59" s="226"/>
-      <c r="F59" s="227"/>
-      <c r="G59" s="227"/>
+      <c r="C59" s="180"/>
+      <c r="D59" s="180"/>
+      <c r="E59" s="180"/>
+      <c r="F59" s="181"/>
+      <c r="G59" s="181"/>
       <c r="H59" s="78"/>
       <c r="I59" s="78"/>
       <c r="J59" s="78"/>
@@ -6973,18 +6973,75 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="97">
-    <mergeCell ref="D34:E35"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="B36:K36"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="D52:F52"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G21:I21"/>
@@ -7001,75 +7058,18 @@
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="A48:K48"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="B36:K36"/>
-    <mergeCell ref="F34:K34"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <conditionalFormatting sqref="F35:K35">
     <cfRule type="expression" dxfId="4" priority="5">
@@ -7661,35 +7661,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="277" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="M1" s="278" t="s">
+      <c r="B1" s="277"/>
+      <c r="C1" s="277"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
+      <c r="M1" s="273" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="279"/>
+      <c r="N1" s="274"/>
     </row>
     <row r="2" spans="1:17" ht="23.45">
-      <c r="A2" s="275" t="s">
+      <c r="A2" s="280" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="275"/>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
+      <c r="D2" s="280"/>
+      <c r="E2" s="280"/>
+      <c r="F2" s="280"/>
+      <c r="G2" s="280"/>
+      <c r="H2" s="280"/>
+      <c r="I2" s="280"/>
       <c r="M2" s="123"/>
       <c r="N2" s="124">
         <f>'WARRANTY SERVICE COMPLAINT FORM'!$B$27</f>
@@ -7703,17 +7703,17 @@
       <c r="A3" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="276" t="str">
+      <c r="B3" s="270" t="str">
         <f>IF('WARRANTY SERVICE COMPLAINT FORM'!$B$11="","",'WARRANTY SERVICE COMPLAINT FORM'!$B$11)</f>
         <v/>
       </c>
-      <c r="C3" s="276"/>
-      <c r="D3" s="276"/>
-      <c r="E3" s="276"/>
-      <c r="F3" s="276"/>
-      <c r="G3" s="276"/>
-      <c r="H3" s="276"/>
-      <c r="I3" s="276"/>
+      <c r="C3" s="270"/>
+      <c r="D3" s="270"/>
+      <c r="E3" s="270"/>
+      <c r="F3" s="270"/>
+      <c r="G3" s="270"/>
+      <c r="H3" s="270"/>
+      <c r="I3" s="270"/>
       <c r="M3" s="125"/>
       <c r="N3" s="126">
         <f>'WARRANTY SERVICE COMPLAINT FORM'!$I$27</f>
@@ -7725,17 +7725,17 @@
       <c r="A4" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="274" t="str">
+      <c r="B4" s="279" t="str">
         <f>CONCATENATE(IF(Data!A33=TRUE,'WARRANTY SERVICE COMPLAINT FORM'!$B27&amp;", ",""),IF(Data!A34=TRUE,'WARRANTY SERVICE COMPLAINT FORM'!$I27&amp;", ",""),IF(Data!A35=TRUE,'WARRANTY SERVICE COMPLAINT FORM'!$B32&amp;", ",""),IF(Data!A36=TRUE,'WARRANTY SERVICE COMPLAINT FORM'!$I32&amp;", ", ""))</f>
         <v/>
       </c>
-      <c r="C4" s="274"/>
-      <c r="D4" s="274"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="274"/>
-      <c r="G4" s="274"/>
-      <c r="H4" s="274"/>
-      <c r="I4" s="274"/>
+      <c r="C4" s="279"/>
+      <c r="D4" s="279"/>
+      <c r="E4" s="279"/>
+      <c r="F4" s="279"/>
+      <c r="G4" s="279"/>
+      <c r="H4" s="279"/>
+      <c r="I4" s="279"/>
       <c r="M4" s="125"/>
       <c r="N4" s="126">
         <f>'WARRANTY SERVICE COMPLAINT FORM'!$B$32</f>
@@ -7747,17 +7747,17 @@
       <c r="A5" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="276" t="str">
+      <c r="B5" s="270" t="str">
         <f>IF('WARRANTY SERVICE COMPLAINT FORM'!B36:K36="","",'WARRANTY SERVICE COMPLAINT FORM'!B36:K36)</f>
         <v/>
       </c>
-      <c r="C5" s="276"/>
-      <c r="D5" s="276"/>
-      <c r="E5" s="276"/>
-      <c r="F5" s="276"/>
-      <c r="G5" s="276"/>
-      <c r="H5" s="276"/>
-      <c r="I5" s="276"/>
+      <c r="C5" s="270"/>
+      <c r="D5" s="270"/>
+      <c r="E5" s="270"/>
+      <c r="F5" s="270"/>
+      <c r="G5" s="270"/>
+      <c r="H5" s="270"/>
+      <c r="I5" s="270"/>
       <c r="M5" s="127"/>
       <c r="N5" s="128">
         <f>'WARRANTY SERVICE COMPLAINT FORM'!$I$32</f>
@@ -7786,13 +7786,13 @@
       <c r="H7" s="117"/>
     </row>
     <row r="8" spans="1:17" ht="39.75" customHeight="1">
-      <c r="A8" s="274" t="s">
+      <c r="A8" s="279" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="274"/>
-      <c r="C8" s="274"/>
-      <c r="D8" s="274"/>
-      <c r="E8" s="274"/>
+      <c r="B8" s="279"/>
+      <c r="C8" s="279"/>
+      <c r="D8" s="279"/>
+      <c r="E8" s="279"/>
       <c r="F8" s="306" t="s">
         <v>68</v>
       </c>
@@ -7802,65 +7802,65 @@
       <c r="P8" s="122"/>
     </row>
     <row r="9" spans="1:17" ht="39.75" customHeight="1">
-      <c r="A9" s="274" t="s">
+      <c r="A9" s="279" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="274"/>
-      <c r="C9" s="274"/>
-      <c r="D9" s="274"/>
-      <c r="E9" s="274"/>
+      <c r="B9" s="279"/>
+      <c r="C9" s="279"/>
+      <c r="D9" s="279"/>
+      <c r="E9" s="279"/>
       <c r="F9" s="119" t="s">
         <v>68</v>
       </c>
       <c r="G9" s="119"/>
-      <c r="H9" s="273"/>
-      <c r="I9" s="273"/>
+      <c r="H9" s="278"/>
+      <c r="I9" s="278"/>
     </row>
     <row r="10" spans="1:17" ht="34.5" customHeight="1">
-      <c r="A10" s="274" t="s">
+      <c r="A10" s="279" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="274"/>
-      <c r="C10" s="274"/>
-      <c r="D10" s="274"/>
-      <c r="E10" s="274"/>
+      <c r="B10" s="279"/>
+      <c r="C10" s="279"/>
+      <c r="D10" s="279"/>
+      <c r="E10" s="279"/>
       <c r="F10" s="119" t="s">
         <v>68</v>
       </c>
       <c r="G10" s="119"/>
-      <c r="H10" s="273"/>
-      <c r="I10" s="273"/>
+      <c r="H10" s="278"/>
+      <c r="I10" s="278"/>
     </row>
     <row r="11" spans="1:17" ht="29.25" customHeight="1">
-      <c r="A11" s="274" t="s">
+      <c r="A11" s="279" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="274"/>
-      <c r="C11" s="274"/>
-      <c r="D11" s="274"/>
-      <c r="E11" s="274"/>
+      <c r="B11" s="279"/>
+      <c r="C11" s="279"/>
+      <c r="D11" s="279"/>
+      <c r="E11" s="279"/>
       <c r="F11" s="306" t="s">
         <v>68</v>
       </c>
       <c r="G11" s="306"/>
-      <c r="H11" s="273"/>
-      <c r="I11" s="273"/>
+      <c r="H11" s="278"/>
+      <c r="I11" s="278"/>
     </row>
     <row r="12" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A12" s="276" t="s">
+      <c r="A12" s="270" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="277"/>
-      <c r="C12" s="277"/>
-      <c r="D12" s="277"/>
-      <c r="E12" s="277"/>
-      <c r="F12" s="277"/>
-      <c r="G12" s="277"/>
-      <c r="H12" s="277"/>
-      <c r="I12" s="277"/>
+      <c r="B12" s="271"/>
+      <c r="C12" s="271"/>
+      <c r="D12" s="271"/>
+      <c r="E12" s="271"/>
+      <c r="F12" s="271"/>
+      <c r="G12" s="271"/>
+      <c r="H12" s="271"/>
+      <c r="I12" s="271"/>
     </row>
     <row r="13" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A13" s="276"/>
+      <c r="A13" s="270"/>
       <c r="B13" s="272"/>
       <c r="C13" s="272"/>
       <c r="D13" s="272"/>
@@ -7871,59 +7871,56 @@
       <c r="I13" s="272"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="280" t="s">
+      <c r="A14" s="275" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="280"/>
-      <c r="C14" s="280"/>
-      <c r="D14" s="280"/>
-      <c r="E14" s="280"/>
-      <c r="F14" s="280"/>
-      <c r="G14" s="280"/>
-      <c r="H14" s="280"/>
-      <c r="I14" s="280"/>
+      <c r="B14" s="275"/>
+      <c r="C14" s="275"/>
+      <c r="D14" s="275"/>
+      <c r="E14" s="275"/>
+      <c r="F14" s="275"/>
+      <c r="G14" s="275"/>
+      <c r="H14" s="275"/>
+      <c r="I14" s="275"/>
     </row>
     <row r="15" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A15" s="280"/>
-      <c r="B15" s="280"/>
-      <c r="C15" s="280"/>
-      <c r="D15" s="280"/>
-      <c r="E15" s="280"/>
-      <c r="F15" s="280"/>
-      <c r="G15" s="280"/>
-      <c r="H15" s="280"/>
-      <c r="I15" s="280"/>
+      <c r="A15" s="275"/>
+      <c r="B15" s="275"/>
+      <c r="C15" s="275"/>
+      <c r="D15" s="275"/>
+      <c r="E15" s="275"/>
+      <c r="F15" s="275"/>
+      <c r="G15" s="275"/>
+      <c r="H15" s="275"/>
+      <c r="I15" s="275"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="270" t="s">
+      <c r="A16" s="276" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="270"/>
-      <c r="C16" s="270"/>
-      <c r="D16" s="270"/>
-      <c r="E16" s="270"/>
-      <c r="F16" s="270"/>
-      <c r="G16" s="270"/>
-      <c r="H16" s="270"/>
-      <c r="I16" s="270"/>
+      <c r="B16" s="276"/>
+      <c r="C16" s="276"/>
+      <c r="D16" s="276"/>
+      <c r="E16" s="276"/>
+      <c r="F16" s="276"/>
+      <c r="G16" s="276"/>
+      <c r="H16" s="276"/>
+      <c r="I16" s="276"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="270"/>
-      <c r="B17" s="270"/>
-      <c r="C17" s="270"/>
-      <c r="D17" s="270"/>
-      <c r="E17" s="270"/>
-      <c r="F17" s="270"/>
-      <c r="G17" s="270"/>
-      <c r="H17" s="270"/>
-      <c r="I17" s="270"/>
+      <c r="A17" s="276"/>
+      <c r="B17" s="276"/>
+      <c r="C17" s="276"/>
+      <c r="D17" s="276"/>
+      <c r="E17" s="276"/>
+      <c r="F17" s="276"/>
+      <c r="G17" s="276"/>
+      <c r="H17" s="276"/>
+      <c r="I17" s="276"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:I13"/>
-    <mergeCell ref="M1:N1"/>
     <mergeCell ref="A14:I15"/>
     <mergeCell ref="A16:I17"/>
     <mergeCell ref="A1:J1"/>
@@ -7941,6 +7938,9 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B5:I5"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:I13"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:J1" location="'WARRANTY SERVICE COMPLAINT FORM'!A1" display="Return to Form" xr:uid="{E00C7E5E-B1C7-4AD5-8A2C-684B9B5ADFF9}"/>
@@ -8061,18 +8061,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="277" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
+      <c r="B1" s="277"/>
+      <c r="C1" s="277"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
     </row>
     <row r="2" spans="1:12" ht="12.95">
       <c r="A2" s="307"/>
@@ -8100,7 +8100,7 @@
       <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="281" t="s">
+      <c r="A4" s="294" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="308"/>
@@ -8145,69 +8145,69 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" s="26"/>
-      <c r="C9" s="285"/>
-      <c r="D9" s="285"/>
-      <c r="E9" s="285"/>
-      <c r="F9" s="285"/>
+      <c r="C9" s="298"/>
+      <c r="D9" s="298"/>
+      <c r="E9" s="298"/>
+      <c r="F9" s="298"/>
       <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="282">
+      <c r="C10" s="295">
         <f xml:space="preserve"> 'WARRANTY SERVICE COMPLAINT FORM'!$B$12</f>
         <v>0</v>
       </c>
-      <c r="D10" s="283"/>
-      <c r="E10" s="283"/>
-      <c r="F10" s="284"/>
+      <c r="D10" s="296"/>
+      <c r="E10" s="296"/>
+      <c r="F10" s="297"/>
       <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" s="19"/>
-      <c r="C11" s="282">
+      <c r="C11" s="295">
         <f xml:space="preserve"> 'WARRANTY SERVICE COMPLAINT FORM'!$B$13</f>
         <v>0</v>
       </c>
-      <c r="D11" s="283"/>
-      <c r="E11" s="283"/>
-      <c r="F11" s="284"/>
+      <c r="D11" s="296"/>
+      <c r="E11" s="296"/>
+      <c r="F11" s="297"/>
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" s="19"/>
-      <c r="C12" s="282">
+      <c r="C12" s="295">
         <f xml:space="preserve"> 'WARRANTY SERVICE COMPLAINT FORM'!$B$14</f>
         <v>0</v>
       </c>
-      <c r="D12" s="283"/>
-      <c r="E12" s="283"/>
-      <c r="F12" s="284"/>
+      <c r="D12" s="296"/>
+      <c r="E12" s="296"/>
+      <c r="F12" s="297"/>
       <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" s="19"/>
-      <c r="C13" s="282">
+      <c r="C13" s="295">
         <f xml:space="preserve"> 'WARRANTY SERVICE COMPLAINT FORM'!$B$15</f>
         <v>0</v>
       </c>
-      <c r="D13" s="283"/>
-      <c r="E13" s="283"/>
-      <c r="F13" s="284"/>
+      <c r="D13" s="296"/>
+      <c r="E13" s="296"/>
+      <c r="F13" s="297"/>
       <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:12">
       <c r="B14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="282">
+      <c r="C14" s="295">
         <f xml:space="preserve"> 'WARRANTY SERVICE COMPLAINT FORM'!$B$16</f>
         <v>0</v>
       </c>
-      <c r="D14" s="283"/>
-      <c r="E14" s="283"/>
-      <c r="F14" s="284"/>
+      <c r="D14" s="296"/>
+      <c r="E14" s="296"/>
+      <c r="F14" s="297"/>
       <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:12">
@@ -8272,17 +8272,17 @@
     </row>
     <row r="22" spans="2:12" ht="22.5">
       <c r="B22" s="19"/>
-      <c r="C22" s="297" t="str">
+      <c r="C22" s="292" t="str">
         <f>Data!B17</f>
         <v>____________________</v>
       </c>
-      <c r="D22" s="297"/>
-      <c r="E22" s="297"/>
-      <c r="F22" s="297"/>
-      <c r="G22" s="297"/>
-      <c r="H22" s="297"/>
-      <c r="I22" s="297"/>
-      <c r="J22" s="298"/>
+      <c r="D22" s="292"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="292"/>
+      <c r="G22" s="292"/>
+      <c r="H22" s="292"/>
+      <c r="I22" s="292"/>
+      <c r="J22" s="293"/>
     </row>
     <row r="23" spans="2:12" ht="23.1" thickBot="1">
       <c r="B23" s="19"/>
@@ -8303,12 +8303,12 @@
       <c r="C24" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="292" t="str">
+      <c r="D24" s="287" t="str">
         <f>IF('WARRANTY SERVICE COMPLAINT FORM'!J4="Tech. Cust. Serv. Use", "",'WARRANTY SERVICE COMPLAINT FORM'!J4)</f>
         <v/>
       </c>
-      <c r="E24" s="293"/>
-      <c r="F24" s="294"/>
+      <c r="E24" s="288"/>
+      <c r="F24" s="289"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="J24" s="18"/>
@@ -8330,13 +8330,13 @@
       <c r="J26" s="18"/>
     </row>
     <row r="27" spans="2:12" ht="12.95">
-      <c r="B27" s="295" t="s">
+      <c r="B27" s="290" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="296"/>
-      <c r="D27" s="296"/>
-      <c r="E27" s="296"/>
-      <c r="F27" s="296"/>
+      <c r="C27" s="291"/>
+      <c r="D27" s="291"/>
+      <c r="E27" s="291"/>
+      <c r="F27" s="291"/>
       <c r="J27" s="18"/>
       <c r="L27" s="100"/>
     </row>
@@ -8345,29 +8345,29 @@
       <c r="J28" s="18"/>
     </row>
     <row r="29" spans="2:12" ht="15" customHeight="1">
-      <c r="B29" s="286" t="str">
+      <c r="B29" s="281" t="str">
         <f>IF(Data!A21=TRUE,"**This component has been purged but may still contain residual Chemical or Gas**",IF(Data!A25=TRUE,"**This component has been purged but may still contain residual Chemcial or Gas**",""))</f>
         <v/>
       </c>
-      <c r="C29" s="287"/>
-      <c r="D29" s="287"/>
-      <c r="E29" s="287"/>
-      <c r="F29" s="287"/>
-      <c r="G29" s="287"/>
-      <c r="H29" s="287"/>
-      <c r="I29" s="287"/>
-      <c r="J29" s="288"/>
+      <c r="C29" s="282"/>
+      <c r="D29" s="282"/>
+      <c r="E29" s="282"/>
+      <c r="F29" s="282"/>
+      <c r="G29" s="282"/>
+      <c r="H29" s="282"/>
+      <c r="I29" s="282"/>
+      <c r="J29" s="283"/>
     </row>
     <row r="30" spans="2:12" ht="12.95">
-      <c r="B30" s="289"/>
-      <c r="C30" s="290"/>
-      <c r="D30" s="290"/>
-      <c r="E30" s="290"/>
-      <c r="F30" s="290"/>
-      <c r="G30" s="290"/>
-      <c r="H30" s="290"/>
-      <c r="I30" s="290"/>
-      <c r="J30" s="291"/>
+      <c r="B30" s="284"/>
+      <c r="C30" s="285"/>
+      <c r="D30" s="285"/>
+      <c r="E30" s="285"/>
+      <c r="F30" s="285"/>
+      <c r="G30" s="285"/>
+      <c r="H30" s="285"/>
+      <c r="I30" s="285"/>
+      <c r="J30" s="286"/>
     </row>
     <row r="31" spans="2:12" ht="12.95" thickBot="1">
       <c r="B31" s="17"/>
@@ -8384,17 +8384,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="27">
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="C22:J22"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="C21:J21"/>
@@ -8411,6 +8400,17 @@
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="C22:J22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:J1" location="'WARRANTY SERVICE COMPLAINT FORM'!A1" display="Return to Form" xr:uid="{F9842CA8-C945-4C95-8EDE-61BA7CE59E4D}"/>
@@ -11448,38 +11448,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="1e51cef0-56f6-4662-b0a9-ebedf42e86c8">
-      <UserInfo>
-        <DisplayName>EES Published Content Visitors</DisplayName>
-        <AccountId>362</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Bernard Klees</DisplayName>
-        <AccountId>115</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="15f98810-fb16-4a79-be12-97f6c19ed137">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1e51cef0-56f6-4662-b0a9-ebedf42e86c8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100415ADEBA7C71EC4C9B03FA0A262D2A80" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5b1be8120bdeb1003c57f4ecad29299">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e51cef0-56f6-4662-b0a9-ebedf42e86c8" xmlns:ns3="15f98810-fb16-4a79-be12-97f6c19ed137" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9103782b54da86eb7a833c42584c6193" ns2:_="" ns3:_="">
     <xsd:import namespace="1e51cef0-56f6-4662-b0a9-ebedf42e86c8"/>
@@ -11728,8 +11696,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="1e51cef0-56f6-4662-b0a9-ebedf42e86c8">
+      <UserInfo>
+        <DisplayName>EES Published Content Visitors</DisplayName>
+        <AccountId>362</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Bernard Klees</DisplayName>
+        <AccountId>115</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="15f98810-fb16-4a79-be12-97f6c19ed137">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1e51cef0-56f6-4662-b0a9-ebedf42e86c8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FEA771B-FA26-414B-80AC-95A74B2847B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24E2088F-6D08-489D-983D-AD443958E8D3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11737,5 +11737,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24E2088F-6D08-489D-983D-AD443958E8D3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FEA771B-FA26-414B-80AC-95A74B2847B1}"/>
 </file>
</xml_diff>